<commit_message>
Naming Convention ,TaskList Updated
</commit_message>
<xml_diff>
--- a/TaskList_Team4.xlsx
+++ b/TaskList_Team4.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>S.No</t>
   </si>
@@ -168,6 +168,27 @@
   </si>
   <si>
     <t>Fixing  Alignment in Sign Up and Sign In Pages</t>
+  </si>
+  <si>
+    <t>In List Your Business Page ,need to change image upload button.</t>
+  </si>
+  <si>
+    <t>when using credits in payment page ,it does not updating in myprofile page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heading Spelling Mistake in Offers Page, (background Color should be change)</t>
+  </si>
+  <si>
+    <t>When sign in into MyBusiness page ,it does not navigating to the next page.</t>
+  </si>
+  <si>
+    <t>Sign Up button alignment ,OTP Should be visible only after getting  otp and after that email field should be disable in SignUp ,Sign In Page</t>
+  </si>
+  <si>
+    <t>Location dropdown still showing duplicate Locations.(overrided someone's db)</t>
+  </si>
+  <si>
+    <t>Atharva,Supraja</t>
   </si>
 </sst>
 </file>
@@ -198,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -241,6 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,14 +672,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -672,7 +700,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -682,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -852,7 +880,7 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -915,6 +943,59 @@
       </c>
       <c r="D33" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>44638</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>